<commit_message>
20251225 Many small errors fixed on Small Caps DWREP ETC
</commit_message>
<xml_diff>
--- a/GUI + Reviews/202512/AEX BEL20.xlsx
+++ b/GUI + Reviews/202512/AEX BEL20.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\PM-Indices-IndexOperations\Review Files\202512\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://euronext-my.sharepoint.com/personal/csonneveld_euronext_com/Documents/Documents/Projects/GUI + Reviews/202512/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{86592935-826F-4B04-8E39-A632F6BE676C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{86592935-826F-4B04-8E39-A632F6BE676C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90166B20-4D32-4665-8F79-DFABBFA8EE9A}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{97D8FFA0-1752-4AC3-9155-A85730915DEB}"/>
+    <workbookView xWindow="-29370" yWindow="195" windowWidth="29040" windowHeight="15720" xr2:uid="{97D8FFA0-1752-4AC3-9155-A85730915DEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -471,13 +471,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.00000000000000"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.00000000000000"/>
-    </dxf>
+  <dxfs count="12">
     <dxf>
       <font>
         <b val="0"/>
@@ -798,18 +792,22 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D9A5568D-3875-4C23-92B4-79325EE95101}" name="Table2" displayName="Table2" ref="A1:I51" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" tableBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D9A5568D-3875-4C23-92B4-79325EE95101}" name="Table2" displayName="Table2" ref="A1:I51" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10" tableBorderDxfId="9">
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{5ECC2A37-1E16-479A-9431-01F9DD21C0A5}" name="Rank" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{71D81B62-1FBA-4FC0-909F-32CA2BDB7DC1}" name="Company" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{0D2B3E51-5DD0-453E-B938-53BAE09A1904}" name="ISIN code" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{A91EB049-5D6F-44B7-A2B2-B848FA698F06}" name="MIC" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{DA42209E-037E-4304-9A93-EC7E19010D76}" name="Preliminary number of shares" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{400365A1-43CA-4504-99EC-606404C5DD1F}" name="Preliminary free float" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{871952D4-6A3A-4CAB-A439-2E8075123F2F}" name="Preliminary capping*" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{C20DB35E-98EE-4080-A14C-23893EAFA740}" name="Effective date of review" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{55F29CFD-F1CC-478A-8DEE-B3278294C802}" name="Currency" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{5ECC2A37-1E16-479A-9431-01F9DD21C0A5}" name="Rank" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{71D81B62-1FBA-4FC0-909F-32CA2BDB7DC1}" name="Company" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{0D2B3E51-5DD0-453E-B938-53BAE09A1904}" name="ISIN code" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{A91EB049-5D6F-44B7-A2B2-B848FA698F06}" name="MIC" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{DA42209E-037E-4304-9A93-EC7E19010D76}" name="Preliminary number of shares" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{400365A1-43CA-4504-99EC-606404C5DD1F}" name="Preliminary free float" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{871952D4-6A3A-4CAB-A439-2E8075123F2F}" name="Preliminary capping*" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{C20DB35E-98EE-4080-A14C-23893EAFA740}" name="Effective date of review" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{55F29CFD-F1CC-478A-8DEE-B3278294C802}" name="Currency" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1134,8 +1132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68946480-7B5B-496B-858D-5887114751D2}">
   <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="M41" sqref="M41"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
20251216 WIFRP and a bunch more fixed
</commit_message>
<xml_diff>
--- a/GUI + Reviews/202512/AEX BEL20.xlsx
+++ b/GUI + Reviews/202512/AEX BEL20.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://euronext-my.sharepoint.com/personal/csonneveld_euronext_com/Documents/Documents/Projects/GUI + Reviews/202512/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\PM-Indices-IndexOperations\Review Files\202512\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{86592935-826F-4B04-8E39-A632F6BE676C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90166B20-4D32-4665-8F79-DFABBFA8EE9A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{86592935-826F-4B04-8E39-A632F6BE676C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-29370" yWindow="195" windowWidth="29040" windowHeight="15720" xr2:uid="{97D8FFA0-1752-4AC3-9155-A85730915DEB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{97D8FFA0-1752-4AC3-9155-A85730915DEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -471,7 +471,13 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="14">
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.00000000000000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.00000000000000"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -792,22 +798,18 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D9A5568D-3875-4C23-92B4-79325EE95101}" name="Table2" displayName="Table2" ref="A1:I51" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10" tableBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D9A5568D-3875-4C23-92B4-79325EE95101}" name="Table2" displayName="Table2" ref="A1:I51" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" tableBorderDxfId="11">
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{5ECC2A37-1E16-479A-9431-01F9DD21C0A5}" name="Rank" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{71D81B62-1FBA-4FC0-909F-32CA2BDB7DC1}" name="Company" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{0D2B3E51-5DD0-453E-B938-53BAE09A1904}" name="ISIN code" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{A91EB049-5D6F-44B7-A2B2-B848FA698F06}" name="MIC" dataDxfId="5"/>
-    <tableColumn id="5" xr3:uid="{DA42209E-037E-4304-9A93-EC7E19010D76}" name="Preliminary number of shares" dataDxfId="4"/>
-    <tableColumn id="6" xr3:uid="{400365A1-43CA-4504-99EC-606404C5DD1F}" name="Preliminary free float" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{871952D4-6A3A-4CAB-A439-2E8075123F2F}" name="Preliminary capping*" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{C20DB35E-98EE-4080-A14C-23893EAFA740}" name="Effective date of review" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{55F29CFD-F1CC-478A-8DEE-B3278294C802}" name="Currency" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{5ECC2A37-1E16-479A-9431-01F9DD21C0A5}" name="Rank" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{71D81B62-1FBA-4FC0-909F-32CA2BDB7DC1}" name="Company" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{0D2B3E51-5DD0-453E-B938-53BAE09A1904}" name="ISIN code" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{A91EB049-5D6F-44B7-A2B2-B848FA698F06}" name="MIC" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{DA42209E-037E-4304-9A93-EC7E19010D76}" name="Preliminary number of shares" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{400365A1-43CA-4504-99EC-606404C5DD1F}" name="Preliminary free float" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{871952D4-6A3A-4CAB-A439-2E8075123F2F}" name="Preliminary capping*" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{C20DB35E-98EE-4080-A14C-23893EAFA740}" name="Effective date of review" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{55F29CFD-F1CC-478A-8DEE-B3278294C802}" name="Currency" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1132,8 +1134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68946480-7B5B-496B-858D-5887114751D2}">
   <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="M41" sqref="M41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>